<commit_message>
Add package setup etc.
</commit_message>
<xml_diff>
--- a/categorical_colors.xlsx
+++ b/categorical_colors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ozgeyelekci/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/znicholls/Documents/AGCEC/Misc/ipcc-wg1/colormaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08795EC-A4D6-4744-ADFD-D2C1FDF68684}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1A0380-C225-9547-B444-AC3FE3FB579C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="560" windowWidth="27640" windowHeight="16940" xr2:uid="{5D2234BD-5ABA-9546-8D02-68F27864E536}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16540" xr2:uid="{5D2234BD-5ABA-9546-8D02-68F27864E536}"/>
   </bookViews>
   <sheets>
     <sheet name="categorical" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>red-yellow</t>
   </si>
@@ -63,21 +63,6 @@
     <t>spectrum_cat</t>
   </si>
   <si>
-    <t>2.6</t>
-  </si>
-  <si>
-    <t>4.5</t>
-  </si>
-  <si>
-    <t>6.0</t>
-  </si>
-  <si>
-    <t>8.5</t>
-  </si>
-  <si>
-    <t>RCP</t>
-  </si>
-  <si>
     <t>rcp_cat</t>
   </si>
   <si>
@@ -157,6 +142,18 @@
   </si>
   <si>
     <t>chem_cat</t>
+  </si>
+  <si>
+    <t>rcp85</t>
+  </si>
+  <si>
+    <t>rcp26</t>
+  </si>
+  <si>
+    <t>rcp45</t>
+  </si>
+  <si>
+    <t>rcp60</t>
   </si>
 </sst>
 </file>
@@ -180,7 +177,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -197,15 +194,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,7 +354,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="825500" cy="787400"/>
@@ -962,7 +970,7 @@
   <dimension ref="A1:M73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -973,10 +981,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C1" s="3">
         <v>127</v>
@@ -993,7 +1001,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1">
         <v>173</v>
@@ -1007,7 +1015,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -1021,7 +1029,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -1035,7 +1043,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1">
         <v>102</v>
@@ -1049,7 +1057,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1">
         <v>229</v>
@@ -1063,10 +1071,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C8" s="3">
         <v>30</v>
@@ -1083,7 +1091,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1">
         <v>69</v>
@@ -1097,7 +1105,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1">
         <v>242</v>
@@ -1111,7 +1119,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1">
         <v>232</v>
@@ -1125,7 +1133,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1">
         <v>128</v>
@@ -1139,10 +1147,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C14" s="3">
         <v>30</v>
@@ -1159,7 +1167,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1">
         <v>29</v>
@@ -1173,7 +1181,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1">
         <v>234</v>
@@ -1187,7 +1195,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1">
         <v>242</v>
@@ -1201,7 +1209,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C18" s="1">
         <v>242</v>
@@ -1215,7 +1223,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1">
         <v>99</v>
@@ -1229,7 +1237,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1">
         <v>232</v>
@@ -1243,7 +1251,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C21" s="1">
         <v>154</v>
@@ -1257,7 +1265,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C22" s="1">
         <v>132</v>
@@ -1274,10 +1282,10 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C24" s="3">
         <v>204</v>
@@ -1294,7 +1302,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C25" s="1">
         <v>37</v>
@@ -1306,73 +1314,71 @@
         <v>204</v>
       </c>
     </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="1">
+        <v>153</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>2</v>
+      </c>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="C28" s="1">
-        <v>153</v>
+        <v>196</v>
       </c>
       <c r="D28" s="1">
+        <v>121</v>
+      </c>
+      <c r="E28" s="1">
         <v>0</v>
-      </c>
-      <c r="E28" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C29" s="1">
-        <v>196</v>
+        <v>112</v>
       </c>
       <c r="D29" s="1">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="E29" s="1">
-        <v>0</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C30" s="1">
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="D30" s="1">
-        <v>160</v>
+        <v>52</v>
       </c>
       <c r="E30" s="1">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0</v>
-      </c>
-      <c r="D31" s="1">
-        <v>52</v>
-      </c>
-      <c r="E31" s="1">
         <v>102</v>
       </c>
     </row>
@@ -1829,6 +1835,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C30:G30 C27:G27 C28:G28 C29:G29" numberStoredAsText="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>